<commit_message>
Getter and setter testing
</commit_message>
<xml_diff>
--- a/testcases-doc/ingredients-logic-test.xlsx
+++ b/testcases-doc/ingredients-logic-test.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zonyyu/Library/Mobile Documents/com~apple~CloudDocs/Documents/University Courses/CMPUT 301/shell379/testcases-doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55FE634-0252-0D44-AE92-DB5F8AC4EA5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B42545E-DED2-E24E-A123-A20A48846548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{F7D94915-29D8-F346-869F-E726E00967C5}"/>
+    <workbookView xWindow="3120" yWindow="2160" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{F7D94915-29D8-F346-869F-E726E00967C5}"/>
   </bookViews>
   <sheets>
     <sheet name="testConstructor" sheetId="1" r:id="rId1"/>
+    <sheet name="setters" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -108,6 +109,42 @@
   </si>
   <si>
     <t>equals(0), "g"</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>setDescription</t>
+  </si>
+  <si>
+    <t>*params</t>
+  </si>
+  <si>
+    <t>""</t>
+  </si>
+  <si>
+    <t>"description"</t>
+  </si>
+  <si>
+    <t>Expected behaviour</t>
+  </si>
+  <si>
+    <t>setBestBefore</t>
+  </si>
+  <si>
+    <t>earlier date</t>
+  </si>
+  <si>
+    <t>later date</t>
+  </si>
+  <si>
+    <t>setLocation</t>
+  </si>
+  <si>
+    <t>"pantry"</t>
   </si>
 </sst>
 </file>
@@ -123,7 +160,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,6 +185,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -161,12 +210,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,7 +533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD265A0C-2174-C64F-AC15-F7E23823D88A}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -702,28 +752,28 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="B9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="4" t="s">
+      <c r="D9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H9" s="4" t="s">
+      <c r="G9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -731,25 +781,11 @@
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -845,6 +881,154 @@
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8493C9EA-D3B3-834C-BDE7-C989818EC591}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="9" max="9" width="22.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>